<commit_message>
refactor: ajuste na planilha modelo
</commit_message>
<xml_diff>
--- a/Resources/PlanilhaFerias-Modelo.xlsx
+++ b/Resources/PlanilhaFerias-Modelo.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://groupsoftware-my.sharepoint.com/personal/guilherme_campos_groupsoftware_com_br/Documents/Área de Trabalho/gerador-periodos/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilherme.campos\OneDrive - Group Software Ltda\Área de Trabalho\gerador-periodos\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{A72CD46B-0074-4E47-BC9D-A9C926E3EF27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB77A18A-7B92-4F4E-BD2A-2CE27A793A9C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72F1C0D-FD9E-41A0-A88B-01CE5C6B6A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{57081FCD-5C37-41D2-84B5-2D9D411D8DA3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{57081FCD-5C37-41D2-84B5-2D9D411D8DA3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Fatos Geradores" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha2" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -35,38 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
-  <si>
-    <t>Férias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dias de férias </t>
-  </si>
-  <si>
-    <t>CpfFuncionario</t>
-  </si>
-  <si>
-    <t>Inicio do periodo Aquisitivo</t>
-  </si>
-  <si>
-    <t>Fim do periodo Aquisitivo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Retorno </t>
-  </si>
-  <si>
-    <t>Data Pagamento</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Status</t>
   </si>
   <si>
-    <t xml:space="preserve">Inicio do gozo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fim do gozo </t>
-  </si>
-  <si>
     <t>Identificador Empresa</t>
   </si>
   <si>
@@ -83,37 +56,22 @@
   </si>
   <si>
     <t>Historica</t>
+  </si>
+  <si>
+    <t>CPF Do Funcionario</t>
+  </si>
+  <si>
+    <t>Data de Admissão</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="7"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -124,19 +82,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -151,30 +111,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -491,82 +439,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2290F624-35B9-4A02-A7A7-6DDBEC61F37D}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A1528" sqref="A3:XFD1528"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" style="5" customWidth="1"/>
-    <col min="11" max="11" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>7</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6FF5B417-2C83-4929-A3A1-34EC8FE18FF6}">
-          <x14:formula1>
-            <xm:f>Planilha2!$B$2:$B$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>J3:J1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -582,32 +484,32 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>